<commit_message>
correctif problème insertion matière dans bd et mise à jour semestre étudiant lors de l'inscription
</commit_message>
<xml_diff>
--- a/projetS5/public/INFO/2018-2019/ADMIN/MATIERES/INFO_2018-2019_ADMIN_MATIERES_S4_PEL.xlsx
+++ b/projetS5/public/INFO/2018-2019/ADMIN/MATIERES/INFO_2018-2019_ADMIN_MATIERES_S4_PEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcde\Music\PROJET S5 LPDIOC GESTION ETUDIANT\GestionEtudiants2018\projetS5\public\INFO\2018-2019\ADMIN\MATIERES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF8E99-B78D-4178-B27B-D96926A0D78D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8896FB-3548-4ABC-851E-756BEF6008CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{59F2304F-887A-4A54-BA91-8630B5535E47}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{59F2304F-887A-4A54-BA91-8630B5535E47}"/>
   </bookViews>
   <sheets>
     <sheet name="Matières" sheetId="1" r:id="rId1"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49AC56B-0BD6-4F52-8FD0-1514D2748A67}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71CB888-873A-4C6E-B364-C00F8F1B15C5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>